<commit_message>
cleanup. prepared for publish
</commit_message>
<xml_diff>
--- a/PlannerOpenXML/Resources/planner.xlsx
+++ b/PlannerOpenXML/Resources/planner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\PlannerOpenXML\PlannerOpenXML\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11616480-A1F1-4EA8-B84A-BE20A72EEFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1D0212-7676-41A7-B295-281280F79D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planner" sheetId="3" r:id="rId1"/>
@@ -783,7 +783,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" zoomScaleSheetLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData/>

</xml_diff>